<commit_message>
Reformated server code for more visibility and added future development point
</commit_message>
<xml_diff>
--- a/Glucids_App/data/Shiny_test.xlsx
+++ b/Glucids_App/data/Shiny_test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdechaumet\Google Drive\Perso\Programming\R\03_Development\Shiny_App_Glucids\Glucids_App\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_Perso\26.Google.Drive\Perso\Programming\R\03_Development\Targeted_tool\Glucids_App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="4455" windowHeight="11505"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="4455" windowHeight="11505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Datamatrix" sheetId="2" r:id="rId1"/>
@@ -524,9 +524,6 @@
     <t>GENERGYE</t>
   </si>
   <si>
-    <t>Conc(µM)</t>
-  </si>
-  <si>
     <t>batch</t>
   </si>
   <si>
@@ -547,11 +544,14 @@
   <si>
     <t>standard</t>
   </si>
+  <si>
+    <t>conc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1557,7 +1557,7 @@
   <tableColumns count="4">
     <tableColumn id="1" name="VariableID"/>
     <tableColumn id="2" name="class"/>
-    <tableColumn id="4" name="Conc(µM)"/>
+    <tableColumn id="4" name="conc"/>
     <tableColumn id="3" name="Unit"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1853,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14547,7 +14547,7 @@
   <dimension ref="A1:O109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J12" sqref="A1:O109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14580,10 +14580,10 @@
         <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>164</v>
@@ -14627,7 +14627,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -14674,7 +14674,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -14721,7 +14721,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -14768,7 +14768,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -14815,7 +14815,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -14862,7 +14862,7 @@
         <v>76</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -14909,7 +14909,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -14956,7 +14956,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -15003,7 +15003,7 @@
         <v>78</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -15050,7 +15050,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -15097,7 +15097,7 @@
         <v>80</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -15144,7 +15144,7 @@
         <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -15191,7 +15191,7 @@
         <v>82</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -15238,7 +15238,7 @@
         <v>83</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -15285,7 +15285,7 @@
         <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -15332,7 +15332,7 @@
         <v>84</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -15379,7 +15379,7 @@
         <v>85</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -15426,7 +15426,7 @@
         <v>86</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -15473,7 +15473,7 @@
         <v>87</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -15520,7 +15520,7 @@
         <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -15567,7 +15567,7 @@
         <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -15614,7 +15614,7 @@
         <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -15661,7 +15661,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -15708,7 +15708,7 @@
         <v>60</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -15755,7 +15755,7 @@
         <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -15802,7 +15802,7 @@
         <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -15849,7 +15849,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -15896,7 +15896,7 @@
         <v>90</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -15943,7 +15943,7 @@
         <v>91</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -15990,7 +15990,7 @@
         <v>92</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -16037,7 +16037,7 @@
         <v>67</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
@@ -16084,7 +16084,7 @@
         <v>93</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -16131,7 +16131,7 @@
         <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -16178,7 +16178,7 @@
         <v>95</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -16225,7 +16225,7 @@
         <v>96</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E36" s="1">
         <v>1</v>
@@ -16272,7 +16272,7 @@
         <v>97</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -16319,7 +16319,7 @@
         <v>98</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -16366,7 +16366,7 @@
         <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -16413,7 +16413,7 @@
         <v>100</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -16460,7 +16460,7 @@
         <v>101</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -16507,7 +16507,7 @@
         <v>102</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -16554,7 +16554,7 @@
         <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -16601,7 +16601,7 @@
         <v>104</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -16648,7 +16648,7 @@
         <v>105</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E45" s="1">
         <v>1</v>
@@ -16695,7 +16695,7 @@
         <v>106</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -16742,7 +16742,7 @@
         <v>107</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -16789,7 +16789,7 @@
         <v>108</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E48" s="1">
         <v>1</v>
@@ -16836,7 +16836,7 @@
         <v>109</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E49" s="1">
         <v>1</v>
@@ -16883,7 +16883,7 @@
         <v>110</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E50" s="1">
         <v>1</v>
@@ -16930,7 +16930,7 @@
         <v>111</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -16977,7 +16977,7 @@
         <v>112</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E52" s="1">
         <v>1</v>
@@ -17024,7 +17024,7 @@
         <v>113</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E53" s="1">
         <v>1</v>
@@ -17071,7 +17071,7 @@
         <v>114</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -17118,7 +17118,7 @@
         <v>115</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -17165,7 +17165,7 @@
         <v>116</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -17212,7 +17212,7 @@
         <v>117</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -17259,7 +17259,7 @@
         <v>118</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E58" s="1">
         <v>1</v>
@@ -17306,7 +17306,7 @@
         <v>119</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -17353,7 +17353,7 @@
         <v>120</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E60" s="1">
         <v>1</v>
@@ -17400,7 +17400,7 @@
         <v>121</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
@@ -17447,7 +17447,7 @@
         <v>122</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
@@ -17494,7 +17494,7 @@
         <v>123</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -17541,7 +17541,7 @@
         <v>124</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -17588,7 +17588,7 @@
         <v>125</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -17635,7 +17635,7 @@
         <v>126</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -17682,7 +17682,7 @@
         <v>127</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E67" s="1">
         <v>1</v>
@@ -17729,7 +17729,7 @@
         <v>128</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E68" s="1">
         <v>1</v>
@@ -17776,7 +17776,7 @@
         <v>129</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E69" s="1">
         <v>1</v>
@@ -17823,7 +17823,7 @@
         <v>130</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E70" s="1">
         <v>1</v>
@@ -17917,7 +17917,7 @@
         <v>37</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -17964,7 +17964,7 @@
         <v>38</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E73" s="1">
         <v>2</v>
@@ -18011,7 +18011,7 @@
         <v>39</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E74" s="1">
         <v>2</v>
@@ -18058,7 +18058,7 @@
         <v>40</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E75" s="1">
         <v>2</v>
@@ -18105,7 +18105,7 @@
         <v>41</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E76" s="1">
         <v>2</v>
@@ -18152,7 +18152,7 @@
         <v>42</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E77" s="1">
         <v>2</v>
@@ -18199,7 +18199,7 @@
         <v>43</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E78" s="1">
         <v>2</v>
@@ -18246,7 +18246,7 @@
         <v>44</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E79" s="1">
         <v>2</v>
@@ -18293,7 +18293,7 @@
         <v>45</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E80" s="1">
         <v>2</v>
@@ -18340,7 +18340,7 @@
         <v>46</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E81" s="1">
         <v>2</v>
@@ -18387,7 +18387,7 @@
         <v>47</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E82" s="1">
         <v>2</v>
@@ -18434,7 +18434,7 @@
         <v>48</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E83" s="1">
         <v>2</v>
@@ -18481,7 +18481,7 @@
         <v>49</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E84" s="1">
         <v>2</v>
@@ -18528,7 +18528,7 @@
         <v>50</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E85" s="1">
         <v>2</v>
@@ -18575,7 +18575,7 @@
         <v>51</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E86" s="1">
         <v>2</v>
@@ -18622,7 +18622,7 @@
         <v>52</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E87" s="1">
         <v>2</v>
@@ -18669,7 +18669,7 @@
         <v>53</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E88" s="1">
         <v>2</v>
@@ -18716,7 +18716,7 @@
         <v>54</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E89" s="1">
         <v>2</v>
@@ -18763,7 +18763,7 @@
         <v>55</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E90" s="1">
         <v>2</v>
@@ -18810,7 +18810,7 @@
         <v>56</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E91" s="1">
         <v>2</v>
@@ -18857,7 +18857,7 @@
         <v>57</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E92" s="1">
         <v>2</v>
@@ -18904,7 +18904,7 @@
         <v>58</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E93" s="1">
         <v>2</v>
@@ -18951,7 +18951,7 @@
         <v>59</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E94" s="1">
         <v>2</v>
@@ -18998,7 +18998,7 @@
         <v>60</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E95" s="1">
         <v>2</v>
@@ -19045,7 +19045,7 @@
         <v>61</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E96" s="1">
         <v>2</v>
@@ -19092,7 +19092,7 @@
         <v>62</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E97" s="1">
         <v>2</v>
@@ -19139,7 +19139,7 @@
         <v>63</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E98" s="1">
         <v>2</v>
@@ -19186,7 +19186,7 @@
         <v>64</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E99" s="1">
         <v>2</v>
@@ -19233,7 +19233,7 @@
         <v>65</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -19280,7 +19280,7 @@
         <v>66</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E101" s="1">
         <v>2</v>
@@ -19327,7 +19327,7 @@
         <v>67</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E102" s="1">
         <v>2</v>
@@ -19374,7 +19374,7 @@
         <v>68</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E103" s="1">
         <v>2</v>
@@ -19421,7 +19421,7 @@
         <v>69</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E104" s="1">
         <v>2</v>
@@ -19468,7 +19468,7 @@
         <v>70</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E105" s="1">
         <v>2</v>
@@ -19515,7 +19515,7 @@
         <v>71</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E106" s="1">
         <v>2</v>
@@ -19562,7 +19562,7 @@
         <v>72</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E107" s="1">
         <v>2</v>
@@ -19609,7 +19609,7 @@
         <v>73</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E108" s="1">
         <v>2</v>
@@ -19704,8 +19704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19720,10 +19720,10 @@
         <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>137</v>

</xml_diff>